<commit_message>
Subir cosas para usar plugin en QGIS
</commit_message>
<xml_diff>
--- a/Lineas.xlsx
+++ b/Lineas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/engineering/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisd\OneDrive\Escritorio\Repos GitHub\GIS_fork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106373AA-FA32-5C45-80AF-6C731F2A2228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAEF213-A4C6-4088-9281-38BFD0F8FFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lineas" sheetId="1" r:id="rId1"/>
@@ -6724,30 +6724,30 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:BQ456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BS456" sqref="BS456"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E444" sqref="E444"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -7538,7 +7538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
       </c>
@@ -8314,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -8508,7 +8508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -8702,7 +8702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>115</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>125</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -9672,7 +9672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>147</v>
       </c>
@@ -9866,7 +9866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>158</v>
       </c>
@@ -10254,7 +10254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>159</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -10642,7 +10642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>170</v>
       </c>
@@ -10836,7 +10836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>180</v>
       </c>
@@ -11224,7 +11224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>188</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>189</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>190</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>194</v>
       </c>
@@ -12000,7 +12000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>204</v>
       </c>
@@ -12194,7 +12194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>212</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>220</v>
       </c>
@@ -12582,7 +12582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>228</v>
       </c>
@@ -12776,7 +12776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>236</v>
       </c>
@@ -12970,7 +12970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -13358,7 +13358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>239</v>
       </c>
@@ -13552,7 +13552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>247</v>
       </c>
@@ -13746,7 +13746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>257</v>
       </c>
@@ -13940,7 +13940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>258</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>259</v>
       </c>
@@ -14328,7 +14328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>268</v>
       </c>
@@ -14522,7 +14522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>269</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>277</v>
       </c>
@@ -14910,7 +14910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>278</v>
       </c>
@@ -15104,7 +15104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>279</v>
       </c>
@@ -15298,7 +15298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>289</v>
       </c>
@@ -15492,7 +15492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>299</v>
       </c>
@@ -15686,7 +15686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>300</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>301</v>
       </c>
@@ -16074,7 +16074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>308</v>
       </c>
@@ -16268,7 +16268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>316</v>
       </c>
@@ -16462,7 +16462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>321</v>
       </c>
@@ -16656,7 +16656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>322</v>
       </c>
@@ -16850,7 +16850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>323</v>
       </c>
@@ -17044,7 +17044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>324</v>
       </c>
@@ -17238,7 +17238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>325</v>
       </c>
@@ -17432,7 +17432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>333</v>
       </c>
@@ -17626,7 +17626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>334</v>
       </c>
@@ -17820,7 +17820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>339</v>
       </c>
@@ -18014,7 +18014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>344</v>
       </c>
@@ -18208,7 +18208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>345</v>
       </c>
@@ -18402,7 +18402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>353</v>
       </c>
@@ -18596,7 +18596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>354</v>
       </c>
@@ -18790,7 +18790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>368</v>
       </c>
@@ -18984,7 +18984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>378</v>
       </c>
@@ -19178,7 +19178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>386</v>
       </c>
@@ -19372,7 +19372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>396</v>
       </c>
@@ -19566,7 +19566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>397</v>
       </c>
@@ -19760,7 +19760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>398</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>399</v>
       </c>
@@ -20148,7 +20148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -20342,7 +20342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>408</v>
       </c>
@@ -20536,7 +20536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>414</v>
       </c>
@@ -20730,7 +20730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>420</v>
       </c>
@@ -20924,7 +20924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>425</v>
       </c>
@@ -21118,7 +21118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>431</v>
       </c>
@@ -21312,7 +21312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>437</v>
       </c>
@@ -21506,7 +21506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>441</v>
       </c>
@@ -21700,7 +21700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>442</v>
       </c>
@@ -21894,7 +21894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>443</v>
       </c>
@@ -22088,7 +22088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>444</v>
       </c>
@@ -22282,7 +22282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>445</v>
       </c>
@@ -22476,7 +22476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>446</v>
       </c>
@@ -22670,7 +22670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>454</v>
       </c>
@@ -22864,7 +22864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>462</v>
       </c>
@@ -23058,7 +23058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>468</v>
       </c>
@@ -23252,7 +23252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>474</v>
       </c>
@@ -23446,7 +23446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>475</v>
       </c>
@@ -23640,7 +23640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>476</v>
       </c>
@@ -23834,7 +23834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>477</v>
       </c>
@@ -24028,7 +24028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>478</v>
       </c>
@@ -24222,7 +24222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>479</v>
       </c>
@@ -24416,7 +24416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>480</v>
       </c>
@@ -24610,7 +24610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>481</v>
       </c>
@@ -24804,7 +24804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>482</v>
       </c>
@@ -24998,7 +24998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>483</v>
       </c>
@@ -25192,7 +25192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>484</v>
       </c>
@@ -25386,7 +25386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>490</v>
       </c>
@@ -25580,7 +25580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>491</v>
       </c>
@@ -25774,7 +25774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>496</v>
       </c>
@@ -25968,7 +25968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>497</v>
       </c>
@@ -26162,7 +26162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>502</v>
       </c>
@@ -26356,7 +26356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>503</v>
       </c>
@@ -26550,7 +26550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>504</v>
       </c>
@@ -26744,7 +26744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>508</v>
       </c>
@@ -26938,7 +26938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>509</v>
       </c>
@@ -27132,7 +27132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>510</v>
       </c>
@@ -27326,7 +27326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>511</v>
       </c>
@@ -27520,7 +27520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>512</v>
       </c>
@@ -27714,7 +27714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>518</v>
       </c>
@@ -27908,7 +27908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>519</v>
       </c>
@@ -28102,7 +28102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>522</v>
       </c>
@@ -28296,7 +28296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>528</v>
       </c>
@@ -28490,7 +28490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>529</v>
       </c>
@@ -28684,7 +28684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>535</v>
       </c>
@@ -28878,7 +28878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>539</v>
       </c>
@@ -29072,7 +29072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>542</v>
       </c>
@@ -29266,7 +29266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>545</v>
       </c>
@@ -29460,7 +29460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>548</v>
       </c>
@@ -29654,7 +29654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1926</v>
       </c>
@@ -29848,7 +29848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1927</v>
       </c>
@@ -30042,7 +30042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1928</v>
       </c>
@@ -30236,7 +30236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1929</v>
       </c>
@@ -30430,7 +30430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1930</v>
       </c>
@@ -30624,7 +30624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1931</v>
       </c>
@@ -30818,7 +30818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1932</v>
       </c>
@@ -31012,7 +31012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>1933</v>
       </c>
@@ -31206,7 +31206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1934</v>
       </c>
@@ -31400,7 +31400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>563</v>
       </c>
@@ -31594,7 +31594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>567</v>
       </c>
@@ -31788,7 +31788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>571</v>
       </c>
@@ -31982,7 +31982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>575</v>
       </c>
@@ -32176,7 +32176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>576</v>
       </c>
@@ -32370,7 +32370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>577</v>
       </c>
@@ -32564,7 +32564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>578</v>
       </c>
@@ -32758,7 +32758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>579</v>
       </c>
@@ -32952,7 +32952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>580</v>
       </c>
@@ -33146,7 +33146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>584</v>
       </c>
@@ -33340,7 +33340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>585</v>
       </c>
@@ -33534,7 +33534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>586</v>
       </c>
@@ -33728,7 +33728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>590</v>
       </c>
@@ -33922,7 +33922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>591</v>
       </c>
@@ -34116,7 +34116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>592</v>
       </c>
@@ -34310,7 +34310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>593</v>
       </c>
@@ -34504,7 +34504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>594</v>
       </c>
@@ -34698,7 +34698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>595</v>
       </c>
@@ -34892,7 +34892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>596</v>
       </c>
@@ -35086,7 +35086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>600</v>
       </c>
@@ -35280,7 +35280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>601</v>
       </c>
@@ -35474,7 +35474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>605</v>
       </c>
@@ -35668,7 +35668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>606</v>
       </c>
@@ -35862,7 +35862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>610</v>
       </c>
@@ -36056,7 +36056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>614</v>
       </c>
@@ -36250,7 +36250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>615</v>
       </c>
@@ -36444,7 +36444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>618</v>
       </c>
@@ -36638,7 +36638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>619</v>
       </c>
@@ -36832,7 +36832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>620</v>
       </c>
@@ -37026,7 +37026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>624</v>
       </c>
@@ -37220,7 +37220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>627</v>
       </c>
@@ -37414,7 +37414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>630</v>
       </c>
@@ -37608,7 +37608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>636</v>
       </c>
@@ -37802,7 +37802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>637</v>
       </c>
@@ -37996,7 +37996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>640</v>
       </c>
@@ -38190,7 +38190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>655</v>
       </c>
@@ -38384,7 +38384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>671</v>
       </c>
@@ -38578,7 +38578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>686</v>
       </c>
@@ -38772,7 +38772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>701</v>
       </c>
@@ -38966,7 +38966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>702</v>
       </c>
@@ -39160,7 +39160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>703</v>
       </c>
@@ -39354,7 +39354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>714</v>
       </c>
@@ -39548,7 +39548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>715</v>
       </c>
@@ -39742,7 +39742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>731</v>
       </c>
@@ -39936,7 +39936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>732</v>
       </c>
@@ -40130,7 +40130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>743</v>
       </c>
@@ -40324,7 +40324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>744</v>
       </c>
@@ -40518,7 +40518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>754</v>
       </c>
@@ -40712,7 +40712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>755</v>
       </c>
@@ -40906,7 +40906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>762</v>
       </c>
@@ -41100,7 +41100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>763</v>
       </c>
@@ -41294,7 +41294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>764</v>
       </c>
@@ -41488,7 +41488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>765</v>
       </c>
@@ -41682,7 +41682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>781</v>
       </c>
@@ -41876,7 +41876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>797</v>
       </c>
@@ -42070,7 +42070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>798</v>
       </c>
@@ -42264,7 +42264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>813</v>
       </c>
@@ -42458,7 +42458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>818</v>
       </c>
@@ -42652,7 +42652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>819</v>
       </c>
@@ -42846,7 +42846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>820</v>
       </c>
@@ -43040,7 +43040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>821</v>
       </c>
@@ -43234,7 +43234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>837</v>
       </c>
@@ -43428,7 +43428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>838</v>
       </c>
@@ -43622,7 +43622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>849</v>
       </c>
@@ -43816,7 +43816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>850</v>
       </c>
@@ -44010,7 +44010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>851</v>
       </c>
@@ -44204,7 +44204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>852</v>
       </c>
@@ -44398,7 +44398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>853</v>
       </c>
@@ -44592,7 +44592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>869</v>
       </c>
@@ -44786,7 +44786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>870</v>
       </c>
@@ -44980,7 +44980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>871</v>
       </c>
@@ -45174,7 +45174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>872</v>
       </c>
@@ -45368,7 +45368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>873</v>
       </c>
@@ -45562,7 +45562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>874</v>
       </c>
@@ -45756,7 +45756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>875</v>
       </c>
@@ -45950,7 +45950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>876</v>
       </c>
@@ -46144,7 +46144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>879</v>
       </c>
@@ -46338,7 +46338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>880</v>
       </c>
@@ -46532,7 +46532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>891</v>
       </c>
@@ -46726,7 +46726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>892</v>
       </c>
@@ -46920,7 +46920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>893</v>
       </c>
@@ -47114,7 +47114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>894</v>
       </c>
@@ -47308,7 +47308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>904</v>
       </c>
@@ -47502,7 +47502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>905</v>
       </c>
@@ -47696,7 +47696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>914</v>
       </c>
@@ -47890,7 +47890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>917</v>
       </c>
@@ -48084,7 +48084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>933</v>
       </c>
@@ -48278,7 +48278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>944</v>
       </c>
@@ -48472,7 +48472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>945</v>
       </c>
@@ -48666,7 +48666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>956</v>
       </c>
@@ -48860,7 +48860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>957</v>
       </c>
@@ -49054,7 +49054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>968</v>
       </c>
@@ -49248,7 +49248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>969</v>
       </c>
@@ -49442,7 +49442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>985</v>
       </c>
@@ -49636,7 +49636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>986</v>
       </c>
@@ -49830,7 +49830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>995</v>
       </c>
@@ -50024,7 +50024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>996</v>
       </c>
@@ -50218,7 +50218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>1012</v>
       </c>
@@ -50412,7 +50412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>1022</v>
       </c>
@@ -50606,7 +50606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>1023</v>
       </c>
@@ -50800,7 +50800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>1034</v>
       </c>
@@ -50994,7 +50994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>1035</v>
       </c>
@@ -51188,7 +51188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>1051</v>
       </c>
@@ -51382,7 +51382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>1067</v>
       </c>
@@ -51576,7 +51576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>1068</v>
       </c>
@@ -51770,7 +51770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>1079</v>
       </c>
@@ -51964,7 +51964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>1080</v>
       </c>
@@ -52158,7 +52158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>1096</v>
       </c>
@@ -52352,7 +52352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>1112</v>
       </c>
@@ -52546,7 +52546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>1124</v>
       </c>
@@ -52740,7 +52740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>1125</v>
       </c>
@@ -52934,7 +52934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>1141</v>
       </c>
@@ -53128,7 +53128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>1157</v>
       </c>
@@ -53322,7 +53322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>1167</v>
       </c>
@@ -53516,7 +53516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>1179</v>
       </c>
@@ -53710,7 +53710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>1195</v>
       </c>
@@ -53904,7 +53904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>1211</v>
       </c>
@@ -54098,7 +54098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>1227</v>
       </c>
@@ -54292,7 +54292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>1228</v>
       </c>
@@ -54486,7 +54486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>1229</v>
       </c>
@@ -54680,7 +54680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>1230</v>
       </c>
@@ -54874,7 +54874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>1239</v>
       </c>
@@ -55068,7 +55068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>1240</v>
       </c>
@@ -55262,7 +55262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>1256</v>
       </c>
@@ -55456,7 +55456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1267</v>
       </c>
@@ -55650,7 +55650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>1283</v>
       </c>
@@ -55844,7 +55844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>1298</v>
       </c>
@@ -56038,7 +56038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>1309</v>
       </c>
@@ -56232,7 +56232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>1310</v>
       </c>
@@ -56426,7 +56426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>1311</v>
       </c>
@@ -56620,7 +56620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>1312</v>
       </c>
@@ -56814,7 +56814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>1317</v>
       </c>
@@ -57008,7 +57008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>1324</v>
       </c>
@@ -57202,7 +57202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>1325</v>
       </c>
@@ -57396,7 +57396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>1326</v>
       </c>
@@ -57590,7 +57590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>1342</v>
       </c>
@@ -57784,7 +57784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>1343</v>
       </c>
@@ -57978,7 +57978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>1359</v>
       </c>
@@ -58172,7 +58172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>1360</v>
       </c>
@@ -58366,7 +58366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>1379</v>
       </c>
@@ -58560,7 +58560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>1395</v>
       </c>
@@ -58754,7 +58754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>1396</v>
       </c>
@@ -58948,7 +58948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>1410</v>
       </c>
@@ -59142,7 +59142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>1411</v>
       </c>
@@ -59336,7 +59336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>1412</v>
       </c>
@@ -59530,7 +59530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>1423</v>
       </c>
@@ -59724,7 +59724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>1424</v>
       </c>
@@ -59918,7 +59918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>1425</v>
       </c>
@@ -60112,7 +60112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>1441</v>
       </c>
@@ -60306,7 +60306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1442</v>
       </c>
@@ -60500,7 +60500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>1443</v>
       </c>
@@ -60694,7 +60694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>1444</v>
       </c>
@@ -60888,7 +60888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>1460</v>
       </c>
@@ -61082,7 +61082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>1467</v>
       </c>
@@ -61276,7 +61276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>1468</v>
       </c>
@@ -61470,7 +61470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>1484</v>
       </c>
@@ -61664,7 +61664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>1485</v>
       </c>
@@ -61858,7 +61858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>1486</v>
       </c>
@@ -62052,7 +62052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>1487</v>
       </c>
@@ -62246,7 +62246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>1500</v>
       </c>
@@ -62440,7 +62440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>1516</v>
       </c>
@@ -62634,7 +62634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>1517</v>
       </c>
@@ -62828,7 +62828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>1518</v>
       </c>
@@ -63022,7 +63022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>1534</v>
       </c>
@@ -63216,7 +63216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>1535</v>
       </c>
@@ -63410,7 +63410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>1551</v>
       </c>
@@ -63604,7 +63604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>1552</v>
       </c>
@@ -63798,7 +63798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>1568</v>
       </c>
@@ -63992,7 +63992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>1584</v>
       </c>
@@ -64186,7 +64186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>1595</v>
       </c>
@@ -64380,7 +64380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>1596</v>
       </c>
@@ -64574,7 +64574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>1597</v>
       </c>
@@ -64768,7 +64768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>1608</v>
       </c>
@@ -64962,7 +64962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>1609</v>
       </c>
@@ -65156,7 +65156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>1610</v>
       </c>
@@ -65350,7 +65350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>1626</v>
       </c>
@@ -65544,7 +65544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>1627</v>
       </c>
@@ -65738,7 +65738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>1628</v>
       </c>
@@ -65932,7 +65932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>1639</v>
       </c>
@@ -66126,7 +66126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>1640</v>
       </c>
@@ -66320,7 +66320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>1649</v>
       </c>
@@ -66514,7 +66514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>1650</v>
       </c>
@@ -66708,7 +66708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>1661</v>
       </c>
@@ -66902,7 +66902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>1677</v>
       </c>
@@ -67096,7 +67096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>1685</v>
       </c>
@@ -67290,7 +67290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>1686</v>
       </c>
@@ -67484,7 +67484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>1697</v>
       </c>
@@ -67678,7 +67678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>1710</v>
       </c>
@@ -67872,7 +67872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>1711</v>
       </c>
@@ -68066,7 +68066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>1712</v>
       </c>
@@ -68260,7 +68260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>1713</v>
       </c>
@@ -68454,7 +68454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>1727</v>
       </c>
@@ -68648,7 +68648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>1733</v>
       </c>
@@ -68842,7 +68842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>1734</v>
       </c>
@@ -69036,7 +69036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>1735</v>
       </c>
@@ -69230,7 +69230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>1737</v>
       </c>
@@ -69424,7 +69424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>1738</v>
       </c>
@@ -69618,7 +69618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>1739</v>
       </c>
@@ -69812,7 +69812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>1740</v>
       </c>
@@ -70006,7 +70006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>1741</v>
       </c>
@@ -70200,7 +70200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>1742</v>
       </c>
@@ -70394,7 +70394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>1743</v>
       </c>
@@ -70588,7 +70588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>1747</v>
       </c>
@@ -70782,7 +70782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>1748</v>
       </c>
@@ -70976,7 +70976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>1749</v>
       </c>
@@ -71170,7 +71170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>1750</v>
       </c>
@@ -71364,7 +71364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>1751</v>
       </c>
@@ -71558,7 +71558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>1755</v>
       </c>
@@ -71752,7 +71752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>1756</v>
       </c>
@@ -71946,7 +71946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>1757</v>
       </c>
@@ -72140,7 +72140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>1758</v>
       </c>
@@ -72334,7 +72334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>1762</v>
       </c>
@@ -72528,7 +72528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>1763</v>
       </c>
@@ -72722,7 +72722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>1764</v>
       </c>
@@ -72916,7 +72916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>1765</v>
       </c>
@@ -73110,7 +73110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>1766</v>
       </c>
@@ -73304,7 +73304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>1767</v>
       </c>
@@ -73498,7 +73498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>1771</v>
       </c>
@@ -73692,7 +73692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>1772</v>
       </c>
@@ -73886,7 +73886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>1773</v>
       </c>
@@ -74080,7 +74080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>1774</v>
       </c>
@@ -74274,7 +74274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>1775</v>
       </c>
@@ -74468,7 +74468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>1776</v>
       </c>
@@ -74662,7 +74662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>1777</v>
       </c>
@@ -74856,7 +74856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>1778</v>
       </c>
@@ -75050,7 +75050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>1782</v>
       </c>
@@ -75244,7 +75244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>1785</v>
       </c>
@@ -75438,7 +75438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>1786</v>
       </c>
@@ -75632,7 +75632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>1787</v>
       </c>
@@ -75826,7 +75826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>1788</v>
       </c>
@@ -76020,7 +76020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>1789</v>
       </c>
@@ -76214,7 +76214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>1790</v>
       </c>
@@ -76408,7 +76408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>1791</v>
       </c>
@@ -76602,7 +76602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>1798</v>
       </c>
@@ -76796,7 +76796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>1799</v>
       </c>
@@ -76990,7 +76990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>1803</v>
       </c>
@@ -77184,7 +77184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>1804</v>
       </c>
@@ -77378,7 +77378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>1805</v>
       </c>
@@ -77572,7 +77572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>1806</v>
       </c>
@@ -77766,7 +77766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>1807</v>
       </c>
@@ -77960,7 +77960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>1808</v>
       </c>
@@ -78154,7 +78154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>1809</v>
       </c>
@@ -78348,7 +78348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>1810</v>
       </c>
@@ -78542,7 +78542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>1811</v>
       </c>
@@ -78736,7 +78736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>1812</v>
       </c>
@@ -78930,7 +78930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>1813</v>
       </c>
@@ -79124,7 +79124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>1814</v>
       </c>
@@ -79318,7 +79318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>1815</v>
       </c>
@@ -79512,7 +79512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>1819</v>
       </c>
@@ -79706,7 +79706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>1820</v>
       </c>
@@ -79900,7 +79900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>1821</v>
       </c>
@@ -80094,7 +80094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>1822</v>
       </c>
@@ -80288,7 +80288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>1823</v>
       </c>
@@ -80482,7 +80482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>1824</v>
       </c>
@@ -80676,7 +80676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>1825</v>
       </c>
@@ -80870,7 +80870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>1829</v>
       </c>
@@ -81064,7 +81064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>1830</v>
       </c>
@@ -81258,7 +81258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>1831</v>
       </c>
@@ -81452,7 +81452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>1832</v>
       </c>
@@ -81646,7 +81646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>1833</v>
       </c>
@@ -81840,7 +81840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>1834</v>
       </c>
@@ -82034,7 +82034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>1835</v>
       </c>
@@ -82228,7 +82228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>1836</v>
       </c>
@@ -82422,7 +82422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>1837</v>
       </c>
@@ -82616,7 +82616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>1838</v>
       </c>
@@ -82810,7 +82810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>1839</v>
       </c>
@@ -83004,7 +83004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>1840</v>
       </c>
@@ -83198,7 +83198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>1841</v>
       </c>
@@ -83392,7 +83392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>1842</v>
       </c>
@@ -83586,7 +83586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>1843</v>
       </c>
@@ -83780,7 +83780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>1844</v>
       </c>
@@ -83974,7 +83974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>1845</v>
       </c>
@@ -84168,7 +84168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>1846</v>
       </c>
@@ -84362,7 +84362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>1847</v>
       </c>
@@ -84556,7 +84556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>1848</v>
       </c>
@@ -84750,7 +84750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>1849</v>
       </c>
@@ -84944,7 +84944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>1850</v>
       </c>
@@ -85138,7 +85138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>1851</v>
       </c>
@@ -85332,7 +85332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>1852</v>
       </c>
@@ -85526,7 +85526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>1853</v>
       </c>
@@ -85720,7 +85720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>1854</v>
       </c>
@@ -85914,7 +85914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>1855</v>
       </c>
@@ -86108,7 +86108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>1856</v>
       </c>
@@ -86302,7 +86302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>1857</v>
       </c>
@@ -86496,7 +86496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>1861</v>
       </c>
@@ -86690,7 +86690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>1862</v>
       </c>
@@ -86884,7 +86884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>1863</v>
       </c>
@@ -87078,7 +87078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>1864</v>
       </c>
@@ -87272,7 +87272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>1865</v>
       </c>
@@ -87466,7 +87466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>1866</v>
       </c>
@@ -87660,7 +87660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>1870</v>
       </c>
@@ -87854,7 +87854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>1879</v>
       </c>
@@ -88048,7 +88048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>1880</v>
       </c>
@@ -88242,7 +88242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>1881</v>
       </c>
@@ -88436,7 +88436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>1935</v>
       </c>
@@ -88630,7 +88630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>1936</v>
       </c>
@@ -88824,7 +88824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>1937</v>
       </c>
@@ -89018,7 +89018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>1938</v>
       </c>
@@ -89212,7 +89212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>1939</v>
       </c>
@@ -89406,7 +89406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>1882</v>
       </c>
@@ -89600,7 +89600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>1883</v>
       </c>
@@ -89794,7 +89794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>1893</v>
       </c>
@@ -89988,7 +89988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>1894</v>
       </c>
@@ -90182,7 +90182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>1895</v>
       </c>
@@ -90376,7 +90376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>1896</v>
       </c>
@@ -90570,7 +90570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>1906</v>
       </c>
@@ -90764,7 +90764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>1907</v>
       </c>
@@ -90958,7 +90958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>1908</v>
       </c>
@@ -91152,7 +91152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>1909</v>
       </c>
@@ -91346,7 +91346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>1910</v>
       </c>
@@ -91540,7 +91540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>1911</v>
       </c>
@@ -91734,7 +91734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>1912</v>
       </c>
@@ -91928,7 +91928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>1913</v>
       </c>
@@ -92122,7 +92122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>1914</v>
       </c>
@@ -92316,7 +92316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>1915</v>
       </c>
@@ -92510,7 +92510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>1916</v>
       </c>
@@ -92704,7 +92704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>1917</v>
       </c>
@@ -92898,7 +92898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>1918</v>
       </c>
@@ -93092,7 +93092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>1919</v>
       </c>
@@ -93286,7 +93286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>1920</v>
       </c>
@@ -93480,7 +93480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>1921</v>
       </c>
@@ -93674,7 +93674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>1922</v>
       </c>
@@ -93868,7 +93868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>1923</v>
       </c>
@@ -94062,7 +94062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>1924</v>
       </c>
@@ -94256,7 +94256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>1925</v>
       </c>
@@ -94450,7 +94450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:69" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>1940</v>
       </c>
@@ -94644,7 +94644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:69" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>1941</v>
       </c>

</xml_diff>